<commit_message>
add new functions in helpers.php
</commit_message>
<xml_diff>
--- a/Components.xlsx
+++ b/Components.xlsx
@@ -1711,7 +1711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1787,29 +1787,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1820,8 +1802,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1836,6 +1833,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2158,16 +2164,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -2196,10 +2202,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="19" t="s">
@@ -2222,8 +2228,8 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="30"/>
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="19" t="s">
         <v>12</v>
       </c>
@@ -2244,8 +2250,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="19" t="s">
         <v>18</v>
       </c>
@@ -2266,9 +2272,9 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="33" t="s">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="34" t="s">
         <v>375</v>
       </c>
       <c r="D6" s="20" t="s">
@@ -2280,17 +2286,17 @@
       <c r="F6" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="30" t="s">
+      <c r="G6" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="32" t="s">
+      <c r="H6" s="35" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="33"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="34"/>
       <c r="D7" s="20" t="s">
         <v>19</v>
       </c>
@@ -2300,13 +2306,13 @@
       <c r="F7" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G7" s="30"/>
-      <c r="H7" s="32"/>
+      <c r="G7" s="36"/>
+      <c r="H7" s="35"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="32" t="s">
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="35" t="s">
         <v>377</v>
       </c>
       <c r="D8" s="20" t="s">
@@ -2318,17 +2324,17 @@
       <c r="F8" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H8" s="32" t="s">
+      <c r="H8" s="35" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="32"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="35"/>
       <c r="D9" s="20" t="s">
         <v>401</v>
       </c>
@@ -2338,12 +2344,12 @@
       <c r="F9" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="32"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="35"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="24" t="s">
         <v>379</v>
       </c>
@@ -2356,16 +2362,16 @@
       <c r="F10" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="32" t="s">
+      <c r="H10" s="35" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
       <c r="C11" s="19"/>
       <c r="D11" s="20" t="s">
         <v>403</v>
@@ -2376,12 +2382,12 @@
       <c r="F11" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="30"/>
-      <c r="H11" s="32"/>
+      <c r="G11" s="36"/>
+      <c r="H11" s="35"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
       <c r="C12" s="24" t="s">
         <v>381</v>
       </c>
@@ -2402,8 +2408,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
       <c r="C13" s="24" t="s">
         <v>383</v>
       </c>
@@ -2424,9 +2430,9 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="32" t="s">
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="35" t="s">
         <v>384</v>
       </c>
       <c r="D14" s="20" t="s">
@@ -2438,17 +2444,17 @@
       <c r="F14" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="32" t="s">
+      <c r="H14" s="35" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="30"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="32"/>
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="20" t="s">
         <v>386</v>
       </c>
@@ -2458,12 +2464,12 @@
       <c r="F15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="30"/>
-      <c r="H15" s="32"/>
+      <c r="G15" s="36"/>
+      <c r="H15" s="35"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="30"/>
-      <c r="B16" s="30"/>
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
       <c r="C16" s="25" t="s">
         <v>408</v>
       </c>
@@ -2484,8 +2490,8 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
       <c r="C17" s="24" t="s">
         <v>387</v>
       </c>
@@ -2506,8 +2512,8 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
       <c r="C18" s="24" t="s">
         <v>388</v>
       </c>
@@ -2528,9 +2534,9 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="33" t="s">
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="34" t="s">
         <v>389</v>
       </c>
       <c r="D19" s="20" t="s">
@@ -2542,17 +2548,17 @@
       <c r="F19" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="30" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="32" t="s">
+      <c r="G19" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>430</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="33"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="20" t="s">
         <v>395</v>
       </c>
@@ -2562,12 +2568,12 @@
       <c r="F20" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="30"/>
-      <c r="H20" s="32"/>
+      <c r="G20" s="36"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
       <c r="C21" s="24" t="s">
         <v>427</v>
       </c>
@@ -2588,9 +2594,9 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="30"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="33" t="s">
+      <c r="A22" s="36"/>
+      <c r="B22" s="36"/>
+      <c r="C22" s="34" t="s">
         <v>390</v>
       </c>
       <c r="D22" s="20" t="s">
@@ -2602,17 +2608,17 @@
       <c r="F22" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="30" t="s">
+      <c r="G22" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H22" s="32" t="s">
+      <c r="H22" s="35" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="33"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="34"/>
       <c r="D23" s="20" t="s">
         <v>396</v>
       </c>
@@ -2622,13 +2628,13 @@
       <c r="F23" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="30"/>
-      <c r="H23" s="32"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="35"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="33" t="s">
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="34" t="s">
         <v>397</v>
       </c>
       <c r="D24" s="20" t="s">
@@ -2640,17 +2646,17 @@
       <c r="F24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="30" t="s">
+      <c r="G24" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="H24" s="32" t="s">
+      <c r="H24" s="35" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="33"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="34"/>
       <c r="D25" s="20" t="s">
         <v>396</v>
       </c>
@@ -2660,12 +2666,12 @@
       <c r="F25" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="30"/>
-      <c r="H25" s="32"/>
+      <c r="G25" s="36"/>
+      <c r="H25" s="35"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
       <c r="C26" s="24" t="s">
         <v>391</v>
       </c>
@@ -2686,8 +2692,8 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="24" t="s">
         <v>392</v>
       </c>
@@ -2708,20 +2714,20 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="30" t="s">
+      <c r="A29" s="36" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="36" t="s">
         <v>33</v>
       </c>
       <c r="C29" s="19" t="s">
@@ -2744,8 +2750,8 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
       <c r="C30" s="19" t="s">
         <v>36</v>
       </c>
@@ -2766,8 +2772,8 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
       <c r="C31" s="19" t="s">
         <v>39</v>
       </c>
@@ -2788,8 +2794,8 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
       <c r="C32" s="19" t="s">
         <v>413</v>
       </c>
@@ -2810,8 +2816,8 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
       <c r="C33" s="19" t="s">
         <v>416</v>
       </c>
@@ -2832,20 +2838,20 @@
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="34"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
-      <c r="H34" s="34"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
+      <c r="H34" s="32"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="30" t="s">
+      <c r="A35" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="36" t="s">
         <v>42</v>
       </c>
       <c r="C35" s="19" t="s">
@@ -2868,8 +2874,8 @@
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="30"/>
-      <c r="B36" s="30"/>
+      <c r="A36" s="36"/>
+      <c r="B36" s="36"/>
       <c r="C36" s="19" t="s">
         <v>44</v>
       </c>
@@ -2890,8 +2896,8 @@
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
       <c r="C37" s="19" t="s">
         <v>45</v>
       </c>
@@ -2912,20 +2918,20 @@
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="34"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
-      <c r="H38" s="34"/>
+      <c r="A38" s="32"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
+      <c r="H38" s="32"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="35" t="s">
+      <c r="A39" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B39" s="29" t="s">
         <v>71</v>
       </c>
       <c r="C39" s="19" t="s">
@@ -2948,8 +2954,8 @@
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="36"/>
-      <c r="B40" s="36"/>
+      <c r="A40" s="30"/>
+      <c r="B40" s="30"/>
       <c r="C40" s="19" t="s">
         <v>73</v>
       </c>
@@ -2970,8 +2976,8 @@
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="36"/>
-      <c r="B41" s="36"/>
+      <c r="A41" s="30"/>
+      <c r="B41" s="30"/>
       <c r="C41" s="19" t="s">
         <v>74</v>
       </c>
@@ -2992,8 +2998,8 @@
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="37"/>
-      <c r="B42" s="37"/>
+      <c r="A42" s="31"/>
+      <c r="B42" s="31"/>
       <c r="C42" s="19" t="s">
         <v>418</v>
       </c>
@@ -3014,20 +3020,20 @@
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="36" t="s">
         <v>83</v>
       </c>
       <c r="C44" s="19" t="s">
@@ -3050,8 +3056,8 @@
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="19" t="s">
         <v>85</v>
       </c>
@@ -3072,8 +3078,8 @@
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
       <c r="C46" s="19" t="s">
         <v>86</v>
       </c>
@@ -3094,20 +3100,20 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="34"/>
-      <c r="B47" s="34"/>
-      <c r="C47" s="34"/>
-      <c r="D47" s="34"/>
-      <c r="E47" s="34"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="34"/>
+      <c r="A47" s="32"/>
+      <c r="B47" s="32"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="32"/>
+      <c r="F47" s="32"/>
+      <c r="G47" s="32"/>
+      <c r="H47" s="32"/>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="35" t="s">
+      <c r="A48" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="36" t="s">
         <v>95</v>
       </c>
       <c r="C48" s="19" t="s">
@@ -3130,8 +3136,8 @@
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="36"/>
-      <c r="B49" s="30"/>
+      <c r="A49" s="30"/>
+      <c r="B49" s="36"/>
       <c r="C49" s="19" t="s">
         <v>97</v>
       </c>
@@ -3152,8 +3158,8 @@
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="36"/>
-      <c r="B50" s="30"/>
+      <c r="A50" s="30"/>
+      <c r="B50" s="36"/>
       <c r="C50" s="19" t="s">
         <v>98</v>
       </c>
@@ -3174,8 +3180,8 @@
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="37"/>
-      <c r="B51" s="30"/>
+      <c r="A51" s="31"/>
+      <c r="B51" s="36"/>
       <c r="C51" s="19" t="s">
         <v>103</v>
       </c>
@@ -3196,20 +3202,20 @@
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="34"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
-      <c r="H52" s="34"/>
+      <c r="A52" s="32"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
+      <c r="H52" s="32"/>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="30" t="s">
+      <c r="A53" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="36" t="s">
         <v>106</v>
       </c>
       <c r="C53" s="19" t="s">
@@ -3232,8 +3238,8 @@
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="36"/>
       <c r="C54" s="19" t="s">
         <v>108</v>
       </c>
@@ -3254,8 +3260,8 @@
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="36"/>
       <c r="C55" s="19" t="s">
         <v>109</v>
       </c>
@@ -3276,20 +3282,20 @@
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="34"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
-      <c r="H56" s="34"/>
+      <c r="A56" s="32"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
+      <c r="H56" s="32"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="30" t="s">
+      <c r="A57" s="36" t="s">
         <v>114</v>
       </c>
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="36" t="s">
         <v>115</v>
       </c>
       <c r="C57" s="19" t="s">
@@ -3312,8 +3318,8 @@
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="30"/>
-      <c r="B58" s="30"/>
+      <c r="A58" s="36"/>
+      <c r="B58" s="36"/>
       <c r="C58" s="19" t="s">
         <v>117</v>
       </c>
@@ -3334,8 +3340,8 @@
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="36"/>
       <c r="C59" s="19" t="s">
         <v>118</v>
       </c>
@@ -3356,20 +3362,20 @@
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="34"/>
-      <c r="B60" s="34"/>
-      <c r="C60" s="34"/>
-      <c r="D60" s="34"/>
-      <c r="E60" s="34"/>
-      <c r="F60" s="34"/>
-      <c r="G60" s="34"/>
-      <c r="H60" s="34"/>
+      <c r="A60" s="32"/>
+      <c r="B60" s="32"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
+      <c r="E60" s="32"/>
+      <c r="F60" s="32"/>
+      <c r="G60" s="32"/>
+      <c r="H60" s="32"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="30" t="s">
+      <c r="A61" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="36" t="s">
         <v>180</v>
       </c>
       <c r="C61" s="19" t="s">
@@ -3392,9 +3398,9 @@
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="33" t="s">
+      <c r="A62" s="36"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="34" t="s">
         <v>182</v>
       </c>
       <c r="D62" s="20" t="s">
@@ -3414,9 +3420,9 @@
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63" s="30"/>
-      <c r="B63" s="30"/>
-      <c r="C63" s="33"/>
+      <c r="A63" s="36"/>
+      <c r="B63" s="36"/>
+      <c r="C63" s="34"/>
       <c r="D63" s="20" t="s">
         <v>185</v>
       </c>
@@ -3430,8 +3436,8 @@
       <c r="H63" s="22"/>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" s="30"/>
-      <c r="B64" s="30"/>
+      <c r="A64" s="36"/>
+      <c r="B64" s="36"/>
       <c r="C64" s="19" t="s">
         <v>183</v>
       </c>
@@ -3452,20 +3458,20 @@
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" s="34"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="34"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="34"/>
-      <c r="F65" s="34"/>
-      <c r="G65" s="34"/>
-      <c r="H65" s="34"/>
+      <c r="A65" s="32"/>
+      <c r="B65" s="32"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
+      <c r="E65" s="32"/>
+      <c r="F65" s="32"/>
+      <c r="G65" s="32"/>
+      <c r="H65" s="32"/>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" s="30" t="s">
+      <c r="A66" s="36" t="s">
         <v>240</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="36" t="s">
         <v>241</v>
       </c>
       <c r="C66" s="19" t="s">
@@ -3488,8 +3494,8 @@
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
-      <c r="B67" s="30"/>
+      <c r="A67" s="36"/>
+      <c r="B67" s="36"/>
       <c r="C67" s="19" t="s">
         <v>243</v>
       </c>
@@ -3510,8 +3516,8 @@
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
-      <c r="B68" s="30"/>
+      <c r="A68" s="36"/>
+      <c r="B68" s="36"/>
       <c r="C68" s="19" t="s">
         <v>244</v>
       </c>
@@ -3532,20 +3538,20 @@
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="34"/>
-      <c r="H69" s="34"/>
+      <c r="A69" s="32"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="30" t="s">
+      <c r="A70" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="B70" s="30" t="s">
+      <c r="B70" s="36" t="s">
         <v>248</v>
       </c>
       <c r="C70" s="19" t="s">
@@ -3568,8 +3574,8 @@
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
-      <c r="B71" s="30"/>
+      <c r="A71" s="36"/>
+      <c r="B71" s="36"/>
       <c r="C71" s="19" t="s">
         <v>250</v>
       </c>
@@ -3590,8 +3596,8 @@
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="30"/>
-      <c r="B72" s="30"/>
+      <c r="A72" s="36"/>
+      <c r="B72" s="36"/>
       <c r="C72" s="19" t="s">
         <v>251</v>
       </c>
@@ -3612,20 +3618,20 @@
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" s="34"/>
-      <c r="B73" s="34"/>
-      <c r="C73" s="34"/>
-      <c r="D73" s="34"/>
-      <c r="E73" s="34"/>
-      <c r="F73" s="34"/>
-      <c r="G73" s="34"/>
-      <c r="H73" s="34"/>
+      <c r="A73" s="32"/>
+      <c r="B73" s="32"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="32"/>
+      <c r="G73" s="32"/>
+      <c r="H73" s="32"/>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" s="30" t="s">
+      <c r="A74" s="36" t="s">
         <v>258</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="36" t="s">
         <v>259</v>
       </c>
       <c r="C74" s="19" t="s">
@@ -3648,8 +3654,8 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
-      <c r="B75" s="30"/>
+      <c r="A75" s="36"/>
+      <c r="B75" s="36"/>
       <c r="C75" s="19" t="s">
         <v>261</v>
       </c>
@@ -3670,8 +3676,8 @@
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
-      <c r="B76" s="30"/>
+      <c r="A76" s="36"/>
+      <c r="B76" s="36"/>
       <c r="C76" s="19" t="s">
         <v>262</v>
       </c>
@@ -3692,20 +3698,20 @@
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="34"/>
-      <c r="B77" s="34"/>
-      <c r="C77" s="34"/>
-      <c r="D77" s="34"/>
-      <c r="E77" s="34"/>
-      <c r="F77" s="34"/>
-      <c r="G77" s="34"/>
-      <c r="H77" s="34"/>
+      <c r="A77" s="32"/>
+      <c r="B77" s="32"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
+      <c r="E77" s="32"/>
+      <c r="F77" s="32"/>
+      <c r="G77" s="32"/>
+      <c r="H77" s="32"/>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="35" t="s">
+      <c r="A78" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="B78" s="35" t="s">
+      <c r="B78" s="29" t="s">
         <v>274</v>
       </c>
       <c r="C78" s="19" t="s">
@@ -3728,8 +3734,8 @@
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="36"/>
-      <c r="B79" s="36"/>
+      <c r="A79" s="30"/>
+      <c r="B79" s="30"/>
       <c r="C79" s="19" t="s">
         <v>272</v>
       </c>
@@ -3750,8 +3756,8 @@
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" s="36"/>
-      <c r="B80" s="36"/>
+      <c r="A80" s="30"/>
+      <c r="B80" s="30"/>
       <c r="C80" s="19" t="s">
         <v>273</v>
       </c>
@@ -3772,8 +3778,8 @@
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="36"/>
-      <c r="B81" s="36"/>
+      <c r="A81" s="30"/>
+      <c r="B81" s="30"/>
       <c r="C81" s="19" t="s">
         <v>420</v>
       </c>
@@ -3794,8 +3800,8 @@
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="36"/>
-      <c r="B82" s="36"/>
+      <c r="A82" s="30"/>
+      <c r="B82" s="30"/>
       <c r="C82" s="19" t="s">
         <v>421</v>
       </c>
@@ -3816,8 +3822,8 @@
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="37"/>
-      <c r="B83" s="37"/>
+      <c r="A83" s="31"/>
+      <c r="B83" s="31"/>
       <c r="C83" s="19" t="s">
         <v>423</v>
       </c>
@@ -3838,20 +3844,20 @@
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
-      <c r="B84" s="34"/>
-      <c r="C84" s="34"/>
-      <c r="D84" s="34"/>
-      <c r="E84" s="34"/>
-      <c r="F84" s="34"/>
-      <c r="G84" s="34"/>
-      <c r="H84" s="34"/>
+      <c r="A84" s="32"/>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="32"/>
+      <c r="G84" s="32"/>
+      <c r="H84" s="32"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="30" t="s">
+      <c r="A85" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B85" s="36" t="s">
         <v>277</v>
       </c>
       <c r="C85" s="19" t="s">
@@ -3874,9 +3880,9 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="32" t="s">
+      <c r="A86" s="36"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="35" t="s">
         <v>279</v>
       </c>
       <c r="D86" s="20" t="s">
@@ -3888,17 +3894,17 @@
       <c r="F86" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G86" s="30" t="s">
+      <c r="G86" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="H86" s="32" t="s">
+      <c r="H86" s="35" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="32"/>
+      <c r="A87" s="36"/>
+      <c r="B87" s="36"/>
+      <c r="C87" s="35"/>
       <c r="D87" s="20" t="s">
         <v>185</v>
       </c>
@@ -3908,13 +3914,13 @@
       <c r="F87" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G87" s="30"/>
-      <c r="H87" s="32"/>
+      <c r="G87" s="36"/>
+      <c r="H87" s="35"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="32"/>
+      <c r="A88" s="36"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="35"/>
       <c r="D88" s="20" t="s">
         <v>281</v>
       </c>
@@ -3924,12 +3930,12 @@
       <c r="F88" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="G88" s="30"/>
-      <c r="H88" s="32"/>
+      <c r="G88" s="36"/>
+      <c r="H88" s="35"/>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
-      <c r="B89" s="30"/>
+      <c r="A89" s="36"/>
+      <c r="B89" s="36"/>
       <c r="C89" s="19" t="s">
         <v>280</v>
       </c>
@@ -3950,20 +3956,20 @@
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
-      <c r="B90" s="34"/>
-      <c r="C90" s="34"/>
-      <c r="D90" s="34"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="34"/>
-      <c r="G90" s="34"/>
-      <c r="H90" s="34"/>
+      <c r="A90" s="32"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="32"/>
+      <c r="G90" s="32"/>
+      <c r="H90" s="32"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="30" t="s">
+      <c r="A91" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="B91" s="30" t="s">
+      <c r="B91" s="36" t="s">
         <v>286</v>
       </c>
       <c r="C91" s="19" t="s">
@@ -3986,9 +3992,9 @@
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="32" t="s">
+      <c r="A92" s="36"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="35" t="s">
         <v>288</v>
       </c>
       <c r="D92" s="20" t="s">
@@ -4008,9 +4014,9 @@
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
-      <c r="B93" s="30"/>
-      <c r="C93" s="32"/>
+      <c r="A93" s="36"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="35"/>
       <c r="D93" s="20" t="s">
         <v>291</v>
       </c>
@@ -4024,9 +4030,9 @@
       <c r="H93" s="22"/>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="32"/>
+      <c r="A94" s="36"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="35"/>
       <c r="D94" s="20" t="s">
         <v>292</v>
       </c>
@@ -4040,8 +4046,8 @@
       <c r="H94" s="22"/>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
-      <c r="B95" s="30"/>
+      <c r="A95" s="36"/>
+      <c r="B95" s="36"/>
       <c r="C95" s="19" t="s">
         <v>289</v>
       </c>
@@ -4062,17 +4068,72 @@
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" s="38"/>
-      <c r="B96" s="38"/>
-      <c r="C96" s="38"/>
-      <c r="D96" s="38"/>
-      <c r="E96" s="38"/>
-      <c r="F96" s="38"/>
-      <c r="G96" s="38"/>
-      <c r="H96" s="38"/>
+      <c r="A96" s="33"/>
+      <c r="B96" s="33"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="33"/>
+      <c r="F96" s="33"/>
+      <c r="G96" s="33"/>
+      <c r="H96" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="71">
+    <mergeCell ref="B44:B46"/>
+    <mergeCell ref="B48:B51"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A44:A46"/>
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="G6:G7"/>
+    <mergeCell ref="B57:B59"/>
+    <mergeCell ref="B66:B68"/>
+    <mergeCell ref="B70:B72"/>
+    <mergeCell ref="A57:A59"/>
+    <mergeCell ref="A53:A55"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="B53:B55"/>
+    <mergeCell ref="B91:B95"/>
+    <mergeCell ref="A91:A95"/>
+    <mergeCell ref="A65:H65"/>
+    <mergeCell ref="A69:H69"/>
+    <mergeCell ref="A73:H73"/>
+    <mergeCell ref="A77:H77"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A70:A72"/>
+    <mergeCell ref="H86:H88"/>
+    <mergeCell ref="G86:G88"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="A66:A68"/>
+    <mergeCell ref="B74:B76"/>
+    <mergeCell ref="B85:B89"/>
+    <mergeCell ref="H6:H7"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="B3:B27"/>
+    <mergeCell ref="A3:A27"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="H19:H20"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A34:H34"/>
+    <mergeCell ref="A38:H38"/>
+    <mergeCell ref="B35:B37"/>
+    <mergeCell ref="B29:B33"/>
     <mergeCell ref="A39:A42"/>
     <mergeCell ref="B39:B42"/>
     <mergeCell ref="A84:H84"/>
@@ -4089,61 +4150,6 @@
     <mergeCell ref="C62:C63"/>
     <mergeCell ref="C86:C88"/>
     <mergeCell ref="C92:C94"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="A34:H34"/>
-    <mergeCell ref="A38:H38"/>
-    <mergeCell ref="B35:B37"/>
-    <mergeCell ref="H6:H7"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="B3:B27"/>
-    <mergeCell ref="A3:A27"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="B91:B95"/>
-    <mergeCell ref="A91:A95"/>
-    <mergeCell ref="A65:H65"/>
-    <mergeCell ref="A69:H69"/>
-    <mergeCell ref="A73:H73"/>
-    <mergeCell ref="A77:H77"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="H86:H88"/>
-    <mergeCell ref="G86:G88"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="A66:A68"/>
-    <mergeCell ref="B74:B76"/>
-    <mergeCell ref="B85:B89"/>
-    <mergeCell ref="B57:B59"/>
-    <mergeCell ref="B66:B68"/>
-    <mergeCell ref="B70:B72"/>
-    <mergeCell ref="A57:A59"/>
-    <mergeCell ref="A53:A55"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="H19:H20"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="B53:B55"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="B44:B46"/>
-    <mergeCell ref="B48:B51"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="A44:A46"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="G6:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4154,8 +4160,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B43" workbookViewId="0">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4224,10 +4230,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="39" t="s">
+      <c r="A5" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="35" t="s">
         <v>50</v>
       </c>
       <c r="C5" s="19" t="s">
@@ -4247,8 +4253,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="40"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="39"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="19" t="s">
         <v>52</v>
       </c>
@@ -4262,8 +4268,8 @@
       <c r="G6" s="19"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="40"/>
-      <c r="B7" s="32"/>
+      <c r="A7" s="39"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="19" t="s">
         <v>53</v>
       </c>
@@ -4277,8 +4283,8 @@
       <c r="G7" s="19"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="40"/>
-      <c r="B8" s="32"/>
+      <c r="A8" s="39"/>
+      <c r="B8" s="35"/>
       <c r="C8" s="19" t="s">
         <v>54</v>
       </c>
@@ -4292,8 +4298,8 @@
       <c r="G8" s="19"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="32"/>
+      <c r="A9" s="39"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="19" t="s">
         <v>55</v>
       </c>
@@ -4307,8 +4313,8 @@
       <c r="G9" s="19"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="40"/>
-      <c r="B10" s="32"/>
+      <c r="A10" s="39"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="19" t="s">
         <v>56</v>
       </c>
@@ -4322,8 +4328,8 @@
       <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="32"/>
+      <c r="A11" s="39"/>
+      <c r="B11" s="35"/>
       <c r="C11" s="19" t="s">
         <v>57</v>
       </c>
@@ -4337,8 +4343,8 @@
       <c r="G11" s="19"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="40"/>
-      <c r="B12" s="32"/>
+      <c r="A12" s="39"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="19" t="s">
         <v>58</v>
       </c>
@@ -4352,8 +4358,8 @@
       <c r="G12" s="19"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="40"/>
-      <c r="B13" s="32"/>
+      <c r="A13" s="39"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="19" t="s">
         <v>67</v>
       </c>
@@ -4367,16 +4373,16 @@
       <c r="G13" s="19"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="40"/>
-      <c r="B14" s="34"/>
-      <c r="C14" s="34"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="34"/>
-      <c r="F14" s="34"/>
-      <c r="G14" s="34"/>
+      <c r="A14" s="39"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="40"/>
+      <c r="A15" s="39"/>
       <c r="B15" s="19" t="s">
         <v>59</v>
       </c>
@@ -4397,16 +4403,16 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="40"/>
-      <c r="B16" s="34"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
-      <c r="G16" s="34"/>
+      <c r="A16" s="39"/>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
+      <c r="A17" s="39"/>
       <c r="B17" s="19" t="s">
         <v>60</v>
       </c>
@@ -4427,16 +4433,16 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="40"/>
-      <c r="B18" s="34"/>
-      <c r="C18" s="34"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
-      <c r="G18" s="34"/>
+      <c r="A18" s="39"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="40"/>
+      <c r="A19" s="39"/>
       <c r="B19" s="19" t="s">
         <v>80</v>
       </c>
@@ -4457,16 +4463,16 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="40"/>
-      <c r="B20" s="34"/>
-      <c r="C20" s="34"/>
-      <c r="D20" s="34"/>
-      <c r="E20" s="34"/>
-      <c r="F20" s="34"/>
-      <c r="G20" s="34"/>
+      <c r="A20" s="39"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="40"/>
+      <c r="A21" s="39"/>
       <c r="B21" s="19" t="s">
         <v>62</v>
       </c>
@@ -4487,16 +4493,16 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="40"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
+      <c r="A22" s="39"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="40"/>
+      <c r="A23" s="39"/>
       <c r="B23" s="19" t="s">
         <v>91</v>
       </c>
@@ -4517,16 +4523,16 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="40"/>
-      <c r="B24" s="34"/>
-      <c r="C24" s="34"/>
-      <c r="D24" s="34"/>
-      <c r="E24" s="34"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="34"/>
+      <c r="A24" s="39"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="40"/>
+      <c r="A25" s="39"/>
       <c r="B25" s="19" t="s">
         <v>506</v>
       </c>
@@ -4547,16 +4553,16 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="40"/>
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
-      <c r="E26" s="34"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="34"/>
+      <c r="A26" s="39"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="40"/>
+      <c r="A27" s="39"/>
       <c r="B27" s="19" t="s">
         <v>123</v>
       </c>
@@ -4577,16 +4583,16 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
+      <c r="A28" s="39"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="40"/>
+      <c r="A29" s="39"/>
       <c r="B29" s="19" t="s">
         <v>297</v>
       </c>
@@ -4607,16 +4613,16 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="40"/>
-      <c r="B30" s="34"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="34"/>
-      <c r="E30" s="34"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="34"/>
+      <c r="A30" s="39"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="40"/>
+      <c r="A31" s="39"/>
       <c r="B31" s="19" t="s">
         <v>298</v>
       </c>
@@ -4637,16 +4643,16 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="40"/>
-      <c r="B32" s="34"/>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
+      <c r="A32" s="39"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="40"/>
+      <c r="A33" s="39"/>
       <c r="B33" s="19" t="s">
         <v>300</v>
       </c>
@@ -4667,16 +4673,16 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="40"/>
-      <c r="B34" s="34"/>
-      <c r="C34" s="34"/>
-      <c r="D34" s="34"/>
-      <c r="E34" s="34"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="34"/>
+      <c r="A34" s="39"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="40"/>
+      <c r="A35" s="39"/>
       <c r="B35" s="19" t="s">
         <v>301</v>
       </c>
@@ -4697,16 +4703,16 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="40"/>
-      <c r="B36" s="34"/>
-      <c r="C36" s="34"/>
-      <c r="D36" s="34"/>
-      <c r="E36" s="34"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="34"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+      <c r="G36" s="32"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="40"/>
+      <c r="A37" s="39"/>
       <c r="B37" s="19" t="s">
         <v>302</v>
       </c>
@@ -4727,16 +4733,16 @@
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="40"/>
-      <c r="B38" s="34"/>
-      <c r="C38" s="34"/>
-      <c r="D38" s="34"/>
-      <c r="E38" s="34"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="34"/>
+      <c r="A38" s="39"/>
+      <c r="B38" s="32"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="32"/>
+      <c r="F38" s="32"/>
+      <c r="G38" s="32"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="40"/>
+      <c r="A39" s="39"/>
       <c r="B39" s="19" t="s">
         <v>306</v>
       </c>
@@ -4757,16 +4763,16 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="40"/>
-      <c r="B40" s="34"/>
-      <c r="C40" s="34"/>
-      <c r="D40" s="34"/>
-      <c r="E40" s="34"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
+      <c r="A40" s="39"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="32"/>
+      <c r="G40" s="32"/>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" s="40"/>
+      <c r="A41" s="39"/>
       <c r="B41" s="19" t="s">
         <v>308</v>
       </c>
@@ -4787,16 +4793,16 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="40"/>
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="D42" s="34"/>
-      <c r="E42" s="34"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
+      <c r="A42" s="39"/>
+      <c r="B42" s="32"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="32"/>
+      <c r="F42" s="32"/>
+      <c r="G42" s="32"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="40"/>
+      <c r="A43" s="39"/>
       <c r="B43" s="19" t="s">
         <v>310</v>
       </c>
@@ -4817,16 +4823,16 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="40"/>
-      <c r="B44" s="34"/>
-      <c r="C44" s="34"/>
-      <c r="D44" s="34"/>
-      <c r="E44" s="34"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
+      <c r="A44" s="39"/>
+      <c r="B44" s="32"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
+      <c r="F44" s="32"/>
+      <c r="G44" s="32"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="40"/>
+      <c r="A45" s="39"/>
       <c r="B45" s="19" t="s">
         <v>312</v>
       </c>
@@ -4847,16 +4853,16 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="40"/>
-      <c r="B46" s="34"/>
-      <c r="C46" s="34"/>
-      <c r="D46" s="34"/>
-      <c r="E46" s="34"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
+      <c r="A46" s="39"/>
+      <c r="B46" s="32"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="32"/>
+      <c r="G46" s="32"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="40"/>
+      <c r="A47" s="39"/>
       <c r="B47" s="19" t="s">
         <v>314</v>
       </c>
@@ -4877,16 +4883,16 @@
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="40"/>
-      <c r="B48" s="34"/>
-      <c r="C48" s="34"/>
-      <c r="D48" s="34"/>
-      <c r="E48" s="34"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
+      <c r="A48" s="39"/>
+      <c r="B48" s="32"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="32"/>
+      <c r="F48" s="32"/>
+      <c r="G48" s="32"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="40"/>
+      <c r="A49" s="39"/>
       <c r="B49" s="19" t="s">
         <v>316</v>
       </c>
@@ -4907,16 +4913,16 @@
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="40"/>
-      <c r="B50" s="34"/>
-      <c r="C50" s="34"/>
-      <c r="D50" s="34"/>
-      <c r="E50" s="34"/>
-      <c r="F50" s="34"/>
-      <c r="G50" s="34"/>
+      <c r="A50" s="39"/>
+      <c r="B50" s="32"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="32"/>
+      <c r="F50" s="32"/>
+      <c r="G50" s="32"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="40"/>
+      <c r="A51" s="39"/>
       <c r="B51" s="19" t="s">
         <v>91</v>
       </c>
@@ -4937,16 +4943,16 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="40"/>
-      <c r="B52" s="34"/>
-      <c r="C52" s="34"/>
-      <c r="D52" s="34"/>
-      <c r="E52" s="34"/>
-      <c r="F52" s="34"/>
-      <c r="G52" s="34"/>
+      <c r="A52" s="39"/>
+      <c r="B52" s="32"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="32"/>
+      <c r="G52" s="32"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="40"/>
+      <c r="A53" s="39"/>
       <c r="B53" s="19" t="s">
         <v>451</v>
       </c>
@@ -4967,16 +4973,16 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="40"/>
-      <c r="B54" s="34"/>
-      <c r="C54" s="34"/>
-      <c r="D54" s="34"/>
-      <c r="E54" s="34"/>
-      <c r="F54" s="34"/>
-      <c r="G54" s="34"/>
+      <c r="A54" s="39"/>
+      <c r="B54" s="32"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="32"/>
+      <c r="F54" s="32"/>
+      <c r="G54" s="32"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="40"/>
+      <c r="A55" s="39"/>
       <c r="B55" s="19" t="s">
         <v>453</v>
       </c>
@@ -4997,16 +5003,16 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="40"/>
-      <c r="B56" s="34"/>
-      <c r="C56" s="34"/>
-      <c r="D56" s="34"/>
-      <c r="E56" s="34"/>
-      <c r="F56" s="34"/>
-      <c r="G56" s="34"/>
+      <c r="A56" s="39"/>
+      <c r="B56" s="32"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="32"/>
+      <c r="G56" s="32"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="40"/>
+      <c r="A57" s="39"/>
       <c r="B57" s="22" t="s">
         <v>507</v>
       </c>
@@ -5027,16 +5033,16 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="40"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="26"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="26"/>
-      <c r="G58" s="26"/>
+      <c r="A58" s="39"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="45"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="45"/>
+      <c r="G58" s="44"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="40"/>
+      <c r="A59" s="39"/>
       <c r="B59" s="22" t="s">
         <v>510</v>
       </c>
@@ -5057,16 +5063,16 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="40"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="26"/>
-      <c r="D60" s="26"/>
-      <c r="E60" s="26"/>
-      <c r="F60" s="26"/>
-      <c r="G60" s="26"/>
+      <c r="A60" s="39"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="45"/>
+      <c r="D60" s="45"/>
+      <c r="E60" s="45"/>
+      <c r="F60" s="45"/>
+      <c r="G60" s="44"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="41"/>
+      <c r="A61" s="40"/>
       <c r="B61" s="19" t="s">
         <v>456</v>
       </c>
@@ -5088,14 +5094,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="B52:G52"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B42:G42"/>
-    <mergeCell ref="B44:G44"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B50:G50"/>
     <mergeCell ref="B5:B13"/>
     <mergeCell ref="A5:A61"/>
     <mergeCell ref="B14:G14"/>
@@ -5112,6 +5110,14 @@
     <mergeCell ref="B36:G36"/>
     <mergeCell ref="B38:G38"/>
     <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B52:G52"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B42:G42"/>
+    <mergeCell ref="B44:G44"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B50:G50"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5138,17 +5144,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="5"/>
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
@@ -5158,17 +5164,17 @@
       <c r="P1" s="5"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>126</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
       <c r="J2" s="5"/>
       <c r="K2" s="5"/>
       <c r="L2" s="5"/>
@@ -5184,7 +5190,7 @@
       <c r="B3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="28" t="s">
         <v>128</v>
       </c>
       <c r="D3" s="10" t="s">
@@ -5207,13 +5213,13 @@
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
+      <c r="A4" s="36">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="36" t="s">
         <v>458</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="29" t="s">
         <v>369</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -5236,10 +5242,10 @@
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="28" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="27" t="s">
         <v>131</v>
       </c>
       <c r="E5" s="19" t="s">
@@ -5259,9 +5265,9 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="36"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="30"/>
       <c r="D6" s="19" t="s">
         <v>132</v>
       </c>
@@ -5282,9 +5288,9 @@
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="36"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="19" t="s">
         <v>133</v>
       </c>
@@ -5305,9 +5311,9 @@
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="36"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="30"/>
       <c r="D8" s="19" t="s">
         <v>135</v>
       </c>
@@ -5328,9 +5334,9 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="30"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="36"/>
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="30"/>
       <c r="D9" s="19" t="s">
         <v>165</v>
       </c>
@@ -5351,9 +5357,9 @@
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="30"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="36"/>
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="30"/>
       <c r="D10" s="19" t="s">
         <v>167</v>
       </c>
@@ -5374,9 +5380,9 @@
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="36"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="30"/>
       <c r="D11" s="19" t="s">
         <v>435</v>
       </c>
@@ -5397,9 +5403,9 @@
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="36"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="30"/>
       <c r="D12" s="19" t="s">
         <v>437</v>
       </c>
@@ -5420,9 +5426,9 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="36"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="30"/>
       <c r="D13" s="19" t="s">
         <v>505</v>
       </c>
@@ -5443,9 +5449,9 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="37"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="31"/>
       <c r="D14" s="19" t="s">
         <v>439</v>
       </c>
@@ -5466,24 +5472,24 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="36">
         <v>2</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="36" t="s">
         <v>459</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="29" t="s">
         <v>139</v>
       </c>
       <c r="D16" s="19" t="s">
@@ -5506,9 +5512,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="36"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="30"/>
       <c r="D17" s="19" t="s">
         <v>131</v>
       </c>
@@ -5529,9 +5535,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="36"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="30"/>
       <c r="D18" s="19" t="s">
         <v>132</v>
       </c>
@@ -5552,9 +5558,9 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="36"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="30"/>
       <c r="D19" s="19" t="s">
         <v>133</v>
       </c>
@@ -5575,9 +5581,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="36"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="30"/>
       <c r="D20" s="19" t="s">
         <v>135</v>
       </c>
@@ -5598,9 +5604,9 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="30"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="37"/>
+      <c r="A21" s="36"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="31"/>
       <c r="D21" s="19" t="s">
         <v>441</v>
       </c>
@@ -5621,24 +5627,24 @@
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="34"/>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
+      <c r="A23" s="36">
         <v>3</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="36" t="s">
         <v>460</v>
       </c>
-      <c r="C23" s="35" t="s">
+      <c r="C23" s="29" t="s">
         <v>142</v>
       </c>
       <c r="D23" s="19" t="s">
@@ -5661,9 +5667,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="36"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="30"/>
       <c r="D24" s="19" t="s">
         <v>131</v>
       </c>
@@ -5684,9 +5690,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="36"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="30"/>
       <c r="D25" s="19" t="s">
         <v>132</v>
       </c>
@@ -5707,9 +5713,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="36"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="30"/>
       <c r="D26" s="19" t="s">
         <v>133</v>
       </c>
@@ -5730,9 +5736,9 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="30"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="37"/>
+      <c r="A27" s="36"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="31"/>
       <c r="D27" s="19" t="s">
         <v>135</v>
       </c>
@@ -5753,24 +5759,24 @@
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="34"/>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
-      <c r="D28" s="34"/>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
-      <c r="I28" s="34"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="30">
+      <c r="A29" s="36">
         <v>4</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="36" t="s">
         <v>461</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="29" t="s">
         <v>144</v>
       </c>
       <c r="D29" s="19" t="s">
@@ -5793,9 +5799,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="36"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="30"/>
       <c r="D30" s="19" t="s">
         <v>131</v>
       </c>
@@ -5816,9 +5822,9 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="36"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="30"/>
       <c r="D31" s="19" t="s">
         <v>132</v>
       </c>
@@ -5839,9 +5845,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="36"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="30"/>
       <c r="D32" s="19" t="s">
         <v>133</v>
       </c>
@@ -5862,9 +5868,9 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="30"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="36"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="30"/>
       <c r="D33" s="19" t="s">
         <v>441</v>
       </c>
@@ -5885,9 +5891,9 @@
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="30"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="37"/>
+      <c r="A34" s="36"/>
+      <c r="B34" s="36"/>
+      <c r="C34" s="31"/>
       <c r="D34" s="19" t="s">
         <v>135</v>
       </c>
@@ -5908,24 +5914,24 @@
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="34"/>
-      <c r="B35" s="34"/>
-      <c r="C35" s="34"/>
-      <c r="D35" s="34"/>
-      <c r="E35" s="34"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="34"/>
-      <c r="H35" s="34"/>
-      <c r="I35" s="34"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="32"/>
+      <c r="I35" s="32"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="30">
+      <c r="A36" s="36">
         <v>5</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="36" t="s">
         <v>462</v>
       </c>
-      <c r="C36" s="35" t="s">
+      <c r="C36" s="29" t="s">
         <v>146</v>
       </c>
       <c r="D36" s="19" t="s">
@@ -5948,9 +5954,9 @@
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="30"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="36"/>
+      <c r="A37" s="36"/>
+      <c r="B37" s="36"/>
+      <c r="C37" s="30"/>
       <c r="D37" s="19" t="s">
         <v>131</v>
       </c>
@@ -5971,9 +5977,9 @@
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="30"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="36"/>
+      <c r="A38" s="36"/>
+      <c r="B38" s="36"/>
+      <c r="C38" s="30"/>
       <c r="D38" s="19" t="s">
         <v>132</v>
       </c>
@@ -5994,9 +6000,9 @@
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="30"/>
-      <c r="B39" s="30"/>
-      <c r="C39" s="36"/>
+      <c r="A39" s="36"/>
+      <c r="B39" s="36"/>
+      <c r="C39" s="30"/>
       <c r="D39" s="19" t="s">
         <v>133</v>
       </c>
@@ -6017,9 +6023,9 @@
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="30"/>
-      <c r="B40" s="30"/>
-      <c r="C40" s="36"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="36"/>
+      <c r="C40" s="30"/>
       <c r="D40" s="19" t="s">
         <v>135</v>
       </c>
@@ -6040,9 +6046,9 @@
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="30"/>
-      <c r="B41" s="30"/>
-      <c r="C41" s="36"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="30"/>
       <c r="D41" s="19" t="s">
         <v>165</v>
       </c>
@@ -6063,9 +6069,9 @@
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="30"/>
-      <c r="B42" s="30"/>
-      <c r="C42" s="37"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="36"/>
+      <c r="C42" s="31"/>
       <c r="D42" s="19" t="s">
         <v>501</v>
       </c>
@@ -6086,24 +6092,24 @@
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="34"/>
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="D43" s="34"/>
-      <c r="E43" s="34"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="34"/>
-      <c r="I43" s="34"/>
+      <c r="A43" s="32"/>
+      <c r="B43" s="32"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="32"/>
+      <c r="G43" s="32"/>
+      <c r="H43" s="32"/>
+      <c r="I43" s="32"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="30">
+      <c r="A44" s="36">
         <v>6</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="36" t="s">
         <v>463</v>
       </c>
-      <c r="C44" s="35" t="s">
+      <c r="C44" s="29" t="s">
         <v>160</v>
       </c>
       <c r="D44" s="19" t="s">
@@ -6126,9 +6132,9 @@
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="30"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="36"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="36"/>
+      <c r="C45" s="30"/>
       <c r="D45" s="19" t="s">
         <v>131</v>
       </c>
@@ -6149,9 +6155,9 @@
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="30"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="36"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="36"/>
+      <c r="C46" s="30"/>
       <c r="D46" s="19" t="s">
         <v>132</v>
       </c>
@@ -6172,9 +6178,9 @@
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="30"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="36"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="36"/>
+      <c r="C47" s="30"/>
       <c r="D47" s="19" t="s">
         <v>133</v>
       </c>
@@ -6195,9 +6201,9 @@
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="30"/>
-      <c r="B48" s="30"/>
-      <c r="C48" s="36"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="30"/>
       <c r="D48" s="19" t="s">
         <v>135</v>
       </c>
@@ -6218,9 +6224,9 @@
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="30"/>
-      <c r="B49" s="30"/>
-      <c r="C49" s="36"/>
+      <c r="A49" s="36"/>
+      <c r="B49" s="36"/>
+      <c r="C49" s="30"/>
       <c r="D49" s="19" t="s">
         <v>165</v>
       </c>
@@ -6241,9 +6247,9 @@
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="30"/>
-      <c r="B50" s="30"/>
-      <c r="C50" s="37"/>
+      <c r="A50" s="36"/>
+      <c r="B50" s="36"/>
+      <c r="C50" s="31"/>
       <c r="D50" s="19" t="s">
         <v>167</v>
       </c>
@@ -6264,24 +6270,24 @@
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="34"/>
-      <c r="B51" s="34"/>
-      <c r="C51" s="34"/>
-      <c r="D51" s="34"/>
-      <c r="E51" s="34"/>
-      <c r="F51" s="34"/>
-      <c r="G51" s="34"/>
-      <c r="H51" s="34"/>
-      <c r="I51" s="34"/>
+      <c r="A51" s="32"/>
+      <c r="B51" s="32"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="32"/>
+      <c r="F51" s="32"/>
+      <c r="G51" s="32"/>
+      <c r="H51" s="32"/>
+      <c r="I51" s="32"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="30">
+      <c r="A52" s="36">
         <v>7</v>
       </c>
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="36" t="s">
         <v>464</v>
       </c>
-      <c r="C52" s="35" t="s">
+      <c r="C52" s="29" t="s">
         <v>170</v>
       </c>
       <c r="D52" s="19" t="s">
@@ -6304,9 +6310,9 @@
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="30"/>
-      <c r="B53" s="30"/>
-      <c r="C53" s="36"/>
+      <c r="A53" s="36"/>
+      <c r="B53" s="36"/>
+      <c r="C53" s="30"/>
       <c r="D53" s="19" t="s">
         <v>131</v>
       </c>
@@ -6327,9 +6333,9 @@
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A54" s="30"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="36"/>
+      <c r="A54" s="36"/>
+      <c r="B54" s="36"/>
+      <c r="C54" s="30"/>
       <c r="D54" s="19" t="s">
         <v>132</v>
       </c>
@@ -6350,9 +6356,9 @@
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A55" s="30"/>
-      <c r="B55" s="30"/>
-      <c r="C55" s="36"/>
+      <c r="A55" s="36"/>
+      <c r="B55" s="36"/>
+      <c r="C55" s="30"/>
       <c r="D55" s="19" t="s">
         <v>133</v>
       </c>
@@ -6373,9 +6379,9 @@
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A56" s="30"/>
-      <c r="B56" s="30"/>
-      <c r="C56" s="37"/>
+      <c r="A56" s="36"/>
+      <c r="B56" s="36"/>
+      <c r="C56" s="31"/>
       <c r="D56" s="19" t="s">
         <v>135</v>
       </c>
@@ -6396,24 +6402,24 @@
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A57" s="34"/>
-      <c r="B57" s="34"/>
-      <c r="C57" s="34"/>
-      <c r="D57" s="34"/>
-      <c r="E57" s="34"/>
-      <c r="F57" s="34"/>
-      <c r="G57" s="34"/>
-      <c r="H57" s="34"/>
-      <c r="I57" s="34"/>
+      <c r="A57" s="32"/>
+      <c r="B57" s="32"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
+      <c r="E57" s="32"/>
+      <c r="F57" s="32"/>
+      <c r="G57" s="32"/>
+      <c r="H57" s="32"/>
+      <c r="I57" s="32"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A58" s="30">
+      <c r="A58" s="36">
         <v>8</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="36" t="s">
         <v>465</v>
       </c>
-      <c r="C58" s="35" t="s">
+      <c r="C58" s="29" t="s">
         <v>129</v>
       </c>
       <c r="D58" s="19" t="s">
@@ -6436,9 +6442,9 @@
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A59" s="30"/>
-      <c r="B59" s="30"/>
-      <c r="C59" s="36"/>
+      <c r="A59" s="36"/>
+      <c r="B59" s="36"/>
+      <c r="C59" s="30"/>
       <c r="D59" s="19" t="s">
         <v>131</v>
       </c>
@@ -6459,9 +6465,9 @@
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A60" s="30"/>
-      <c r="B60" s="30"/>
-      <c r="C60" s="36"/>
+      <c r="A60" s="36"/>
+      <c r="B60" s="36"/>
+      <c r="C60" s="30"/>
       <c r="D60" s="19" t="s">
         <v>132</v>
       </c>
@@ -6482,9 +6488,9 @@
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A61" s="30"/>
-      <c r="B61" s="30"/>
-      <c r="C61" s="36"/>
+      <c r="A61" s="36"/>
+      <c r="B61" s="36"/>
+      <c r="C61" s="30"/>
       <c r="D61" s="19" t="s">
         <v>133</v>
       </c>
@@ -6505,9 +6511,9 @@
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
-      <c r="B62" s="30"/>
-      <c r="C62" s="37"/>
+      <c r="A62" s="36"/>
+      <c r="B62" s="36"/>
+      <c r="C62" s="31"/>
       <c r="D62" s="19" t="s">
         <v>135</v>
       </c>
@@ -6528,24 +6534,24 @@
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A63" s="34"/>
-      <c r="B63" s="34"/>
-      <c r="C63" s="34"/>
-      <c r="D63" s="34"/>
-      <c r="E63" s="34"/>
-      <c r="F63" s="34"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="34"/>
-      <c r="I63" s="34"/>
+      <c r="A63" s="32"/>
+      <c r="B63" s="32"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="32"/>
+      <c r="F63" s="32"/>
+      <c r="G63" s="32"/>
+      <c r="H63" s="32"/>
+      <c r="I63" s="32"/>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A64" s="30">
+      <c r="A64" s="36">
         <v>9</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="36" t="s">
         <v>466</v>
       </c>
-      <c r="C64" s="35" t="s">
+      <c r="C64" s="29" t="s">
         <v>189</v>
       </c>
       <c r="D64" s="19" t="s">
@@ -6568,9 +6574,9 @@
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A65" s="30"/>
-      <c r="B65" s="30"/>
-      <c r="C65" s="36"/>
+      <c r="A65" s="36"/>
+      <c r="B65" s="36"/>
+      <c r="C65" s="30"/>
       <c r="D65" s="19" t="s">
         <v>131</v>
       </c>
@@ -6591,9 +6597,9 @@
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A66" s="30"/>
-      <c r="B66" s="30"/>
-      <c r="C66" s="36"/>
+      <c r="A66" s="36"/>
+      <c r="B66" s="36"/>
+      <c r="C66" s="30"/>
       <c r="D66" s="19" t="s">
         <v>132</v>
       </c>
@@ -6614,9 +6620,9 @@
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="30"/>
-      <c r="B67" s="30"/>
-      <c r="C67" s="36"/>
+      <c r="A67" s="36"/>
+      <c r="B67" s="36"/>
+      <c r="C67" s="30"/>
       <c r="D67" s="19" t="s">
         <v>133</v>
       </c>
@@ -6637,9 +6643,9 @@
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="30"/>
-      <c r="B68" s="30"/>
-      <c r="C68" s="37"/>
+      <c r="A68" s="36"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="31"/>
       <c r="D68" s="19" t="s">
         <v>135</v>
       </c>
@@ -6660,24 +6666,24 @@
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="34"/>
-      <c r="B69" s="34"/>
-      <c r="C69" s="34"/>
-      <c r="D69" s="34"/>
-      <c r="E69" s="34"/>
-      <c r="F69" s="34"/>
-      <c r="G69" s="34"/>
-      <c r="H69" s="34"/>
-      <c r="I69" s="34"/>
+      <c r="A69" s="32"/>
+      <c r="B69" s="32"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
+      <c r="E69" s="32"/>
+      <c r="F69" s="32"/>
+      <c r="G69" s="32"/>
+      <c r="H69" s="32"/>
+      <c r="I69" s="32"/>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="30">
+      <c r="A70" s="36">
         <v>10</v>
       </c>
-      <c r="B70" s="30" t="s">
+      <c r="B70" s="36" t="s">
         <v>467</v>
       </c>
-      <c r="C70" s="35" t="s">
+      <c r="C70" s="29" t="s">
         <v>319</v>
       </c>
       <c r="D70" s="19" t="s">
@@ -6700,9 +6706,9 @@
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A71" s="30"/>
-      <c r="B71" s="30"/>
-      <c r="C71" s="37"/>
+      <c r="A71" s="36"/>
+      <c r="B71" s="36"/>
+      <c r="C71" s="31"/>
       <c r="D71" s="19" t="s">
         <v>323</v>
       </c>
@@ -6723,24 +6729,24 @@
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A72" s="34"/>
-      <c r="B72" s="34"/>
-      <c r="C72" s="34"/>
-      <c r="D72" s="34"/>
-      <c r="E72" s="34"/>
-      <c r="F72" s="34"/>
-      <c r="G72" s="34"/>
-      <c r="H72" s="34"/>
-      <c r="I72" s="34"/>
+      <c r="A72" s="32"/>
+      <c r="B72" s="32"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="32"/>
+      <c r="G72" s="32"/>
+      <c r="H72" s="32"/>
+      <c r="I72" s="32"/>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A73" s="30">
+      <c r="A73" s="36">
         <v>11</v>
       </c>
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="36" t="s">
         <v>468</v>
       </c>
-      <c r="C73" s="35" t="s">
+      <c r="C73" s="29" t="s">
         <v>325</v>
       </c>
       <c r="D73" s="19" t="s">
@@ -6763,9 +6769,9 @@
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A74" s="30"/>
-      <c r="B74" s="30"/>
-      <c r="C74" s="36"/>
+      <c r="A74" s="36"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="30"/>
       <c r="D74" s="19" t="s">
         <v>131</v>
       </c>
@@ -6786,9 +6792,9 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="30"/>
-      <c r="B75" s="30"/>
-      <c r="C75" s="36"/>
+      <c r="A75" s="36"/>
+      <c r="B75" s="36"/>
+      <c r="C75" s="30"/>
       <c r="D75" s="19" t="s">
         <v>132</v>
       </c>
@@ -6809,9 +6815,9 @@
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A76" s="30"/>
-      <c r="B76" s="30"/>
-      <c r="C76" s="36"/>
+      <c r="A76" s="36"/>
+      <c r="B76" s="36"/>
+      <c r="C76" s="30"/>
       <c r="D76" s="19" t="s">
         <v>133</v>
       </c>
@@ -6832,9 +6838,9 @@
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A77" s="30"/>
-      <c r="B77" s="30"/>
-      <c r="C77" s="37"/>
+      <c r="A77" s="36"/>
+      <c r="B77" s="36"/>
+      <c r="C77" s="31"/>
       <c r="D77" s="19" t="s">
         <v>135</v>
       </c>
@@ -6855,24 +6861,24 @@
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A78" s="34"/>
-      <c r="B78" s="34"/>
-      <c r="C78" s="34"/>
-      <c r="D78" s="34"/>
-      <c r="E78" s="34"/>
-      <c r="F78" s="34"/>
-      <c r="G78" s="34"/>
-      <c r="H78" s="34"/>
-      <c r="I78" s="34"/>
+      <c r="A78" s="32"/>
+      <c r="B78" s="32"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
+      <c r="E78" s="32"/>
+      <c r="F78" s="32"/>
+      <c r="G78" s="32"/>
+      <c r="H78" s="32"/>
+      <c r="I78" s="32"/>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A79" s="30">
+      <c r="A79" s="36">
         <v>12</v>
       </c>
-      <c r="B79" s="30" t="s">
+      <c r="B79" s="36" t="s">
         <v>469</v>
       </c>
-      <c r="C79" s="35" t="s">
+      <c r="C79" s="29" t="s">
         <v>332</v>
       </c>
       <c r="D79" s="19" t="s">
@@ -6895,9 +6901,9 @@
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A80" s="30"/>
-      <c r="B80" s="30"/>
-      <c r="C80" s="36"/>
+      <c r="A80" s="36"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="30"/>
       <c r="D80" s="19" t="s">
         <v>131</v>
       </c>
@@ -6918,9 +6924,9 @@
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A81" s="30"/>
-      <c r="B81" s="30"/>
-      <c r="C81" s="36"/>
+      <c r="A81" s="36"/>
+      <c r="B81" s="36"/>
+      <c r="C81" s="30"/>
       <c r="D81" s="19" t="s">
         <v>132</v>
       </c>
@@ -6941,9 +6947,9 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="30"/>
-      <c r="B82" s="30"/>
-      <c r="C82" s="36"/>
+      <c r="A82" s="36"/>
+      <c r="B82" s="36"/>
+      <c r="C82" s="30"/>
       <c r="D82" s="19" t="s">
         <v>133</v>
       </c>
@@ -6964,9 +6970,9 @@
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A83" s="30"/>
-      <c r="B83" s="30"/>
-      <c r="C83" s="37"/>
+      <c r="A83" s="36"/>
+      <c r="B83" s="36"/>
+      <c r="C83" s="31"/>
       <c r="D83" s="19" t="s">
         <v>135</v>
       </c>
@@ -6987,24 +6993,24 @@
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" s="34"/>
-      <c r="B84" s="34"/>
-      <c r="C84" s="34"/>
-      <c r="D84" s="34"/>
-      <c r="E84" s="34"/>
-      <c r="F84" s="34"/>
-      <c r="G84" s="34"/>
-      <c r="H84" s="34"/>
-      <c r="I84" s="34"/>
+      <c r="A84" s="32"/>
+      <c r="B84" s="32"/>
+      <c r="C84" s="32"/>
+      <c r="D84" s="32"/>
+      <c r="E84" s="32"/>
+      <c r="F84" s="32"/>
+      <c r="G84" s="32"/>
+      <c r="H84" s="32"/>
+      <c r="I84" s="32"/>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A85" s="30">
-        <v>13</v>
-      </c>
-      <c r="B85" s="30" t="s">
+      <c r="A85" s="36">
+        <v>13</v>
+      </c>
+      <c r="B85" s="36" t="s">
         <v>470</v>
       </c>
-      <c r="C85" s="35" t="s">
+      <c r="C85" s="29" t="s">
         <v>339</v>
       </c>
       <c r="D85" s="19" t="s">
@@ -7027,9 +7033,9 @@
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A86" s="30"/>
-      <c r="B86" s="30"/>
-      <c r="C86" s="36"/>
+      <c r="A86" s="36"/>
+      <c r="B86" s="36"/>
+      <c r="C86" s="30"/>
       <c r="D86" s="19" t="s">
         <v>131</v>
       </c>
@@ -7050,9 +7056,9 @@
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A87" s="30"/>
-      <c r="B87" s="30"/>
-      <c r="C87" s="36"/>
+      <c r="A87" s="36"/>
+      <c r="B87" s="36"/>
+      <c r="C87" s="30"/>
       <c r="D87" s="19" t="s">
         <v>132</v>
       </c>
@@ -7073,9 +7079,9 @@
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A88" s="30"/>
-      <c r="B88" s="30"/>
-      <c r="C88" s="36"/>
+      <c r="A88" s="36"/>
+      <c r="B88" s="36"/>
+      <c r="C88" s="30"/>
       <c r="D88" s="19" t="s">
         <v>133</v>
       </c>
@@ -7096,9 +7102,9 @@
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A89" s="30"/>
-      <c r="B89" s="30"/>
-      <c r="C89" s="37"/>
+      <c r="A89" s="36"/>
+      <c r="B89" s="36"/>
+      <c r="C89" s="31"/>
       <c r="D89" s="19" t="s">
         <v>135</v>
       </c>
@@ -7119,24 +7125,24 @@
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A90" s="34"/>
-      <c r="B90" s="34"/>
-      <c r="C90" s="34"/>
-      <c r="D90" s="34"/>
-      <c r="E90" s="34"/>
-      <c r="F90" s="34"/>
-      <c r="G90" s="34"/>
-      <c r="H90" s="34"/>
-      <c r="I90" s="34"/>
+      <c r="A90" s="32"/>
+      <c r="B90" s="32"/>
+      <c r="C90" s="32"/>
+      <c r="D90" s="32"/>
+      <c r="E90" s="32"/>
+      <c r="F90" s="32"/>
+      <c r="G90" s="32"/>
+      <c r="H90" s="32"/>
+      <c r="I90" s="32"/>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A91" s="30">
+      <c r="A91" s="36">
         <v>14</v>
       </c>
-      <c r="B91" s="30" t="s">
+      <c r="B91" s="36" t="s">
         <v>471</v>
       </c>
-      <c r="C91" s="35" t="s">
+      <c r="C91" s="29" t="s">
         <v>340</v>
       </c>
       <c r="D91" s="19" t="s">
@@ -7159,9 +7165,9 @@
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A92" s="30"/>
-      <c r="B92" s="30"/>
-      <c r="C92" s="36"/>
+      <c r="A92" s="36"/>
+      <c r="B92" s="36"/>
+      <c r="C92" s="30"/>
       <c r="D92" s="19" t="s">
         <v>131</v>
       </c>
@@ -7182,9 +7188,9 @@
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A93" s="30"/>
-      <c r="B93" s="30"/>
-      <c r="C93" s="36"/>
+      <c r="A93" s="36"/>
+      <c r="B93" s="36"/>
+      <c r="C93" s="30"/>
       <c r="D93" s="19" t="s">
         <v>132</v>
       </c>
@@ -7205,9 +7211,9 @@
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A94" s="30"/>
-      <c r="B94" s="30"/>
-      <c r="C94" s="36"/>
+      <c r="A94" s="36"/>
+      <c r="B94" s="36"/>
+      <c r="C94" s="30"/>
       <c r="D94" s="19" t="s">
         <v>133</v>
       </c>
@@ -7228,9 +7234,9 @@
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A95" s="30"/>
-      <c r="B95" s="30"/>
-      <c r="C95" s="36"/>
+      <c r="A95" s="36"/>
+      <c r="B95" s="36"/>
+      <c r="C95" s="30"/>
       <c r="D95" s="19" t="s">
         <v>135</v>
       </c>
@@ -7251,9 +7257,9 @@
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A96" s="30"/>
-      <c r="B96" s="30"/>
-      <c r="C96" s="36"/>
+      <c r="A96" s="36"/>
+      <c r="B96" s="36"/>
+      <c r="C96" s="30"/>
       <c r="D96" s="19" t="s">
         <v>485</v>
       </c>
@@ -7274,9 +7280,9 @@
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A97" s="30"/>
-      <c r="B97" s="30"/>
-      <c r="C97" s="37"/>
+      <c r="A97" s="36"/>
+      <c r="B97" s="36"/>
+      <c r="C97" s="31"/>
       <c r="D97" s="19" t="s">
         <v>487</v>
       </c>
@@ -7297,24 +7303,24 @@
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="34"/>
-      <c r="B98" s="34"/>
-      <c r="C98" s="34"/>
-      <c r="D98" s="34"/>
-      <c r="E98" s="34"/>
-      <c r="F98" s="34"/>
-      <c r="G98" s="34"/>
-      <c r="H98" s="34"/>
-      <c r="I98" s="34"/>
+      <c r="A98" s="32"/>
+      <c r="B98" s="32"/>
+      <c r="C98" s="32"/>
+      <c r="D98" s="32"/>
+      <c r="E98" s="32"/>
+      <c r="F98" s="32"/>
+      <c r="G98" s="32"/>
+      <c r="H98" s="32"/>
+      <c r="I98" s="32"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A99" s="30">
-        <v>15</v>
-      </c>
-      <c r="B99" s="30" t="s">
+      <c r="A99" s="36">
+        <v>15</v>
+      </c>
+      <c r="B99" s="36" t="s">
         <v>472</v>
       </c>
-      <c r="C99" s="35" t="s">
+      <c r="C99" s="29" t="s">
         <v>341</v>
       </c>
       <c r="D99" s="19" t="s">
@@ -7337,9 +7343,9 @@
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A100" s="30"/>
-      <c r="B100" s="30"/>
-      <c r="C100" s="36"/>
+      <c r="A100" s="36"/>
+      <c r="B100" s="36"/>
+      <c r="C100" s="30"/>
       <c r="D100" s="19" t="s">
         <v>131</v>
       </c>
@@ -7360,9 +7366,9 @@
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A101" s="30"/>
-      <c r="B101" s="30"/>
-      <c r="C101" s="36"/>
+      <c r="A101" s="36"/>
+      <c r="B101" s="36"/>
+      <c r="C101" s="30"/>
       <c r="D101" s="19" t="s">
         <v>132</v>
       </c>
@@ -7383,9 +7389,9 @@
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A102" s="30"/>
-      <c r="B102" s="30"/>
-      <c r="C102" s="36"/>
+      <c r="A102" s="36"/>
+      <c r="B102" s="36"/>
+      <c r="C102" s="30"/>
       <c r="D102" s="19" t="s">
         <v>133</v>
       </c>
@@ -7406,9 +7412,9 @@
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A103" s="30"/>
-      <c r="B103" s="30"/>
-      <c r="C103" s="37"/>
+      <c r="A103" s="36"/>
+      <c r="B103" s="36"/>
+      <c r="C103" s="31"/>
       <c r="D103" s="19" t="s">
         <v>135</v>
       </c>
@@ -7429,24 +7435,24 @@
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A104" s="34"/>
-      <c r="B104" s="34"/>
-      <c r="C104" s="34"/>
-      <c r="D104" s="34"/>
-      <c r="E104" s="34"/>
-      <c r="F104" s="34"/>
-      <c r="G104" s="34"/>
-      <c r="H104" s="34"/>
-      <c r="I104" s="34"/>
+      <c r="A104" s="32"/>
+      <c r="B104" s="32"/>
+      <c r="C104" s="32"/>
+      <c r="D104" s="32"/>
+      <c r="E104" s="32"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="32"/>
+      <c r="H104" s="32"/>
+      <c r="I104" s="32"/>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A105" s="30">
+      <c r="A105" s="36">
         <v>16</v>
       </c>
-      <c r="B105" s="30" t="s">
+      <c r="B105" s="36" t="s">
         <v>473</v>
       </c>
-      <c r="C105" s="35" t="s">
+      <c r="C105" s="29" t="s">
         <v>342</v>
       </c>
       <c r="D105" s="19" t="s">
@@ -7469,9 +7475,9 @@
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="30"/>
-      <c r="B106" s="30"/>
-      <c r="C106" s="36"/>
+      <c r="A106" s="36"/>
+      <c r="B106" s="36"/>
+      <c r="C106" s="30"/>
       <c r="D106" s="19" t="s">
         <v>131</v>
       </c>
@@ -7492,9 +7498,9 @@
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" s="30"/>
-      <c r="B107" s="30"/>
-      <c r="C107" s="36"/>
+      <c r="A107" s="36"/>
+      <c r="B107" s="36"/>
+      <c r="C107" s="30"/>
       <c r="D107" s="19" t="s">
         <v>132</v>
       </c>
@@ -7515,9 +7521,9 @@
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" s="30"/>
-      <c r="B108" s="30"/>
-      <c r="C108" s="36"/>
+      <c r="A108" s="36"/>
+      <c r="B108" s="36"/>
+      <c r="C108" s="30"/>
       <c r="D108" s="19" t="s">
         <v>133</v>
       </c>
@@ -7538,9 +7544,9 @@
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A109" s="30"/>
-      <c r="B109" s="30"/>
-      <c r="C109" s="36"/>
+      <c r="A109" s="36"/>
+      <c r="B109" s="36"/>
+      <c r="C109" s="30"/>
       <c r="D109" s="19" t="s">
         <v>135</v>
       </c>
@@ -7561,9 +7567,9 @@
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A110" s="30"/>
-      <c r="B110" s="30"/>
-      <c r="C110" s="36"/>
+      <c r="A110" s="36"/>
+      <c r="B110" s="36"/>
+      <c r="C110" s="30"/>
       <c r="D110" s="19" t="s">
         <v>485</v>
       </c>
@@ -7584,9 +7590,9 @@
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A111" s="30"/>
-      <c r="B111" s="30"/>
-      <c r="C111" s="37"/>
+      <c r="A111" s="36"/>
+      <c r="B111" s="36"/>
+      <c r="C111" s="31"/>
       <c r="D111" s="19" t="s">
         <v>489</v>
       </c>
@@ -7607,24 +7613,24 @@
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A112" s="34"/>
-      <c r="B112" s="34"/>
-      <c r="C112" s="34"/>
-      <c r="D112" s="34"/>
-      <c r="E112" s="34"/>
-      <c r="F112" s="34"/>
-      <c r="G112" s="34"/>
-      <c r="H112" s="34"/>
-      <c r="I112" s="34"/>
+      <c r="A112" s="32"/>
+      <c r="B112" s="32"/>
+      <c r="C112" s="32"/>
+      <c r="D112" s="32"/>
+      <c r="E112" s="32"/>
+      <c r="F112" s="32"/>
+      <c r="G112" s="32"/>
+      <c r="H112" s="32"/>
+      <c r="I112" s="32"/>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A113" s="30">
+      <c r="A113" s="36">
         <v>17</v>
       </c>
-      <c r="B113" s="30" t="s">
+      <c r="B113" s="36" t="s">
         <v>474</v>
       </c>
-      <c r="C113" s="35" t="s">
+      <c r="C113" s="29" t="s">
         <v>343</v>
       </c>
       <c r="D113" s="19" t="s">
@@ -7647,9 +7653,9 @@
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A114" s="30"/>
-      <c r="B114" s="30"/>
-      <c r="C114" s="36"/>
+      <c r="A114" s="36"/>
+      <c r="B114" s="36"/>
+      <c r="C114" s="30"/>
       <c r="D114" s="19" t="s">
         <v>131</v>
       </c>
@@ -7670,9 +7676,9 @@
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A115" s="30"/>
-      <c r="B115" s="30"/>
-      <c r="C115" s="36"/>
+      <c r="A115" s="36"/>
+      <c r="B115" s="36"/>
+      <c r="C115" s="30"/>
       <c r="D115" s="19" t="s">
         <v>132</v>
       </c>
@@ -7693,9 +7699,9 @@
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A116" s="30"/>
-      <c r="B116" s="30"/>
-      <c r="C116" s="36"/>
+      <c r="A116" s="36"/>
+      <c r="B116" s="36"/>
+      <c r="C116" s="30"/>
       <c r="D116" s="19" t="s">
         <v>133</v>
       </c>
@@ -7716,9 +7722,9 @@
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A117" s="30"/>
-      <c r="B117" s="30"/>
-      <c r="C117" s="37"/>
+      <c r="A117" s="36"/>
+      <c r="B117" s="36"/>
+      <c r="C117" s="31"/>
       <c r="D117" s="19" t="s">
         <v>135</v>
       </c>
@@ -7739,24 +7745,24 @@
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A118" s="34"/>
-      <c r="B118" s="34"/>
-      <c r="C118" s="34"/>
-      <c r="D118" s="34"/>
-      <c r="E118" s="34"/>
-      <c r="F118" s="34"/>
-      <c r="G118" s="34"/>
-      <c r="H118" s="34"/>
-      <c r="I118" s="34"/>
+      <c r="A118" s="32"/>
+      <c r="B118" s="32"/>
+      <c r="C118" s="32"/>
+      <c r="D118" s="32"/>
+      <c r="E118" s="32"/>
+      <c r="F118" s="32"/>
+      <c r="G118" s="32"/>
+      <c r="H118" s="32"/>
+      <c r="I118" s="32"/>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A119" s="30">
+      <c r="A119" s="36">
         <v>18</v>
       </c>
-      <c r="B119" s="30" t="s">
+      <c r="B119" s="36" t="s">
         <v>491</v>
       </c>
-      <c r="C119" s="35" t="s">
+      <c r="C119" s="29" t="s">
         <v>443</v>
       </c>
       <c r="D119" s="19" t="s">
@@ -7779,9 +7785,9 @@
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A120" s="30"/>
-      <c r="B120" s="30"/>
-      <c r="C120" s="36"/>
+      <c r="A120" s="36"/>
+      <c r="B120" s="36"/>
+      <c r="C120" s="30"/>
       <c r="D120" s="19" t="s">
         <v>131</v>
       </c>
@@ -7802,9 +7808,9 @@
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A121" s="30"/>
-      <c r="B121" s="30"/>
-      <c r="C121" s="36"/>
+      <c r="A121" s="36"/>
+      <c r="B121" s="36"/>
+      <c r="C121" s="30"/>
       <c r="D121" s="19" t="s">
         <v>132</v>
       </c>
@@ -7825,9 +7831,9 @@
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A122" s="30"/>
-      <c r="B122" s="30"/>
-      <c r="C122" s="36"/>
+      <c r="A122" s="36"/>
+      <c r="B122" s="36"/>
+      <c r="C122" s="30"/>
       <c r="D122" s="19" t="s">
         <v>133</v>
       </c>
@@ -7848,9 +7854,9 @@
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A123" s="30"/>
-      <c r="B123" s="30"/>
-      <c r="C123" s="37"/>
+      <c r="A123" s="36"/>
+      <c r="B123" s="36"/>
+      <c r="C123" s="31"/>
       <c r="D123" s="19" t="s">
         <v>135</v>
       </c>
@@ -7871,13 +7877,13 @@
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A125" s="30">
+      <c r="A125" s="36">
         <v>19</v>
       </c>
-      <c r="B125" s="30" t="s">
+      <c r="B125" s="36" t="s">
         <v>475</v>
       </c>
-      <c r="C125" s="35" t="s">
+      <c r="C125" s="29" t="s">
         <v>476</v>
       </c>
       <c r="D125" s="19" t="s">
@@ -7900,9 +7906,9 @@
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A126" s="30"/>
-      <c r="B126" s="30"/>
-      <c r="C126" s="36"/>
+      <c r="A126" s="36"/>
+      <c r="B126" s="36"/>
+      <c r="C126" s="30"/>
       <c r="D126" s="19" t="s">
         <v>478</v>
       </c>
@@ -7923,9 +7929,9 @@
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A127" s="30"/>
-      <c r="B127" s="30"/>
-      <c r="C127" s="37"/>
+      <c r="A127" s="36"/>
+      <c r="B127" s="36"/>
+      <c r="C127" s="31"/>
       <c r="D127" s="19" t="s">
         <v>480</v>
       </c>
@@ -7946,13 +7952,13 @@
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A129" s="27">
+      <c r="A129" s="26">
         <v>20</v>
       </c>
-      <c r="B129" s="27" t="s">
+      <c r="B129" s="26" t="s">
         <v>482</v>
       </c>
-      <c r="C129" s="27" t="s">
+      <c r="C129" s="26" t="s">
         <v>483</v>
       </c>
       <c r="D129" s="19" t="s">
@@ -7975,13 +7981,13 @@
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A131" s="30">
+      <c r="A131" s="36">
         <v>21</v>
       </c>
-      <c r="B131" s="30" t="s">
+      <c r="B131" s="36" t="s">
         <v>492</v>
       </c>
-      <c r="C131" s="35" t="s">
+      <c r="C131" s="29" t="s">
         <v>493</v>
       </c>
       <c r="D131" s="19" t="s">
@@ -8004,9 +8010,9 @@
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A132" s="30"/>
-      <c r="B132" s="30"/>
-      <c r="C132" s="36"/>
+      <c r="A132" s="36"/>
+      <c r="B132" s="36"/>
+      <c r="C132" s="30"/>
       <c r="D132" s="19" t="s">
         <v>495</v>
       </c>
@@ -8027,9 +8033,9 @@
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" s="30"/>
-      <c r="B133" s="30"/>
-      <c r="C133" s="37"/>
+      <c r="A133" s="36"/>
+      <c r="B133" s="36"/>
+      <c r="C133" s="31"/>
       <c r="D133" s="19" t="s">
         <v>496</v>
       </c>
@@ -8051,45 +8057,21 @@
     </row>
   </sheetData>
   <mergeCells count="79">
-    <mergeCell ref="C36:C42"/>
-    <mergeCell ref="C29:C34"/>
-    <mergeCell ref="C125:C127"/>
-    <mergeCell ref="C73:C77"/>
-    <mergeCell ref="B131:B133"/>
-    <mergeCell ref="C131:C133"/>
-    <mergeCell ref="A131:A133"/>
-    <mergeCell ref="A125:A127"/>
-    <mergeCell ref="B125:B127"/>
-    <mergeCell ref="A85:A89"/>
-    <mergeCell ref="A91:A97"/>
-    <mergeCell ref="A99:A103"/>
-    <mergeCell ref="B99:B103"/>
-    <mergeCell ref="A105:A111"/>
-    <mergeCell ref="B105:B111"/>
-    <mergeCell ref="C85:C89"/>
-    <mergeCell ref="C91:C97"/>
-    <mergeCell ref="B79:B83"/>
-    <mergeCell ref="B85:B89"/>
-    <mergeCell ref="B91:B97"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="B70:B71"/>
-    <mergeCell ref="B73:B77"/>
-    <mergeCell ref="A29:A34"/>
-    <mergeCell ref="B29:B34"/>
-    <mergeCell ref="A36:A42"/>
-    <mergeCell ref="B36:B42"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:I2"/>
-    <mergeCell ref="C16:C21"/>
-    <mergeCell ref="A23:A27"/>
-    <mergeCell ref="B23:B27"/>
-    <mergeCell ref="C23:C27"/>
-    <mergeCell ref="A57:I57"/>
-    <mergeCell ref="A51:I51"/>
-    <mergeCell ref="A43:I43"/>
-    <mergeCell ref="A35:I35"/>
-    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="A16:A21"/>
+    <mergeCell ref="B4:B14"/>
+    <mergeCell ref="C4:C14"/>
+    <mergeCell ref="A90:I90"/>
+    <mergeCell ref="A113:A117"/>
+    <mergeCell ref="C99:C103"/>
+    <mergeCell ref="C105:C111"/>
+    <mergeCell ref="C113:C117"/>
+    <mergeCell ref="B113:B117"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="A70:A71"/>
+    <mergeCell ref="A73:A77"/>
+    <mergeCell ref="C79:C83"/>
+    <mergeCell ref="A79:A83"/>
+    <mergeCell ref="C70:C71"/>
     <mergeCell ref="C119:C123"/>
     <mergeCell ref="A119:A123"/>
     <mergeCell ref="A44:A50"/>
@@ -8106,30 +8088,54 @@
     <mergeCell ref="A72:I72"/>
     <mergeCell ref="A69:I69"/>
     <mergeCell ref="A63:I63"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="A73:A77"/>
-    <mergeCell ref="C79:C83"/>
-    <mergeCell ref="A79:A83"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="A118:I118"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="A104:I104"/>
-    <mergeCell ref="A98:I98"/>
-    <mergeCell ref="A90:I90"/>
-    <mergeCell ref="A113:A117"/>
-    <mergeCell ref="C99:C103"/>
-    <mergeCell ref="C105:C111"/>
-    <mergeCell ref="C113:C117"/>
-    <mergeCell ref="B113:B117"/>
+    <mergeCell ref="A29:A34"/>
+    <mergeCell ref="B29:B34"/>
+    <mergeCell ref="A36:A42"/>
+    <mergeCell ref="B36:B42"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:I2"/>
+    <mergeCell ref="C16:C21"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="A35:I35"/>
     <mergeCell ref="A28:I28"/>
     <mergeCell ref="A22:I22"/>
     <mergeCell ref="B16:B21"/>
     <mergeCell ref="A15:I15"/>
     <mergeCell ref="A4:A14"/>
-    <mergeCell ref="A16:A21"/>
-    <mergeCell ref="B4:B14"/>
-    <mergeCell ref="C4:C14"/>
+    <mergeCell ref="A131:A133"/>
+    <mergeCell ref="A125:A127"/>
+    <mergeCell ref="B125:B127"/>
+    <mergeCell ref="A85:A89"/>
+    <mergeCell ref="A91:A97"/>
+    <mergeCell ref="A99:A103"/>
+    <mergeCell ref="B99:B103"/>
+    <mergeCell ref="A105:A111"/>
+    <mergeCell ref="B105:B111"/>
+    <mergeCell ref="B85:B89"/>
+    <mergeCell ref="B91:B97"/>
+    <mergeCell ref="B119:B123"/>
+    <mergeCell ref="A118:I118"/>
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="A104:I104"/>
+    <mergeCell ref="A98:I98"/>
+    <mergeCell ref="C36:C42"/>
+    <mergeCell ref="C29:C34"/>
+    <mergeCell ref="C125:C127"/>
+    <mergeCell ref="C73:C77"/>
+    <mergeCell ref="B131:B133"/>
+    <mergeCell ref="C131:C133"/>
+    <mergeCell ref="C85:C89"/>
+    <mergeCell ref="C91:C97"/>
+    <mergeCell ref="B79:B83"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="B73:B77"/>
+    <mergeCell ref="A57:I57"/>
+    <mergeCell ref="A51:I51"/>
+    <mergeCell ref="A43:I43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8157,30 +8163,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="41" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
+      <c r="I1" s="41"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
@@ -8212,13 +8218,13 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="30">
+      <c r="A4" s="36">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="35" t="s">
         <v>205</v>
       </c>
       <c r="D4" s="19" t="s">
@@ -8241,10 +8247,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="30"/>
-      <c r="C5" s="32"/>
-      <c r="D5" s="28" t="s">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="27" t="s">
         <v>131</v>
       </c>
       <c r="E5" s="19" t="s">
@@ -8264,9 +8270,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="30"/>
-      <c r="C6" s="32"/>
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="35"/>
       <c r="D6" s="19" t="s">
         <v>132</v>
       </c>
@@ -8287,9 +8293,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="30"/>
-      <c r="C7" s="32"/>
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="19" t="s">
         <v>133</v>
       </c>
@@ -8310,9 +8316,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="32"/>
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="35"/>
       <c r="D8" s="19" t="s">
         <v>135</v>
       </c>
@@ -8333,24 +8339,24 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="34"/>
-      <c r="B9" s="34"/>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="32"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="32"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
+      <c r="A10" s="36">
         <v>2</v>
       </c>
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="36" t="s">
         <v>212</v>
       </c>
-      <c r="C10" s="32" t="s">
+      <c r="C10" s="35" t="s">
         <v>212</v>
       </c>
       <c r="D10" s="19" t="s">
@@ -8373,9 +8379,9 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="30"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="32"/>
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="19" t="s">
         <v>131</v>
       </c>
@@ -8396,9 +8402,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="30"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="32"/>
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="19" t="s">
         <v>132</v>
       </c>
@@ -8419,9 +8425,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="30"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="32"/>
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="19" t="s">
         <v>133</v>
       </c>
@@ -8442,9 +8448,9 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="30"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="32"/>
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="19" t="s">
         <v>135</v>
       </c>
@@ -8465,24 +8471,24 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="32"/>
+      <c r="I15" s="32"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="30">
+      <c r="A16" s="36">
         <v>3</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="36" t="s">
         <v>219</v>
       </c>
-      <c r="C16" s="32" t="s">
+      <c r="C16" s="35" t="s">
         <v>219</v>
       </c>
       <c r="D16" s="19" t="s">
@@ -8505,9 +8511,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="30"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="32"/>
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="35"/>
       <c r="D17" s="19" t="s">
         <v>131</v>
       </c>
@@ -8528,9 +8534,9 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="30"/>
-      <c r="B18" s="30"/>
-      <c r="C18" s="32"/>
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="19" t="s">
         <v>132</v>
       </c>
@@ -8551,9 +8557,9 @@
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="30"/>
-      <c r="B19" s="30"/>
-      <c r="C19" s="32"/>
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="19" t="s">
         <v>133</v>
       </c>
@@ -8574,9 +8580,9 @@
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="30"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="32"/>
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="19" t="s">
         <v>135</v>
       </c>
@@ -8597,24 +8603,24 @@
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="34"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="32"/>
+      <c r="I21" s="32"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="A22" s="36">
         <v>4</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="36" t="s">
         <v>226</v>
       </c>
-      <c r="C22" s="32" t="s">
+      <c r="C22" s="35" t="s">
         <v>226</v>
       </c>
       <c r="D22" s="19" t="s">
@@ -8637,9 +8643,9 @@
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="30"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="32"/>
+      <c r="A23" s="36"/>
+      <c r="B23" s="36"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="19" t="s">
         <v>131</v>
       </c>
@@ -8660,9 +8666,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="30"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="32"/>
+      <c r="A24" s="36"/>
+      <c r="B24" s="36"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="19" t="s">
         <v>132</v>
       </c>
@@ -8683,9 +8689,9 @@
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="30"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="32"/>
+      <c r="A25" s="36"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="35"/>
       <c r="D25" s="19" t="s">
         <v>133</v>
       </c>
@@ -8706,9 +8712,9 @@
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="30"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="32"/>
+      <c r="A26" s="36"/>
+      <c r="B26" s="36"/>
+      <c r="C26" s="35"/>
       <c r="D26" s="19" t="s">
         <v>135</v>
       </c>
@@ -8729,24 +8735,24 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="34"/>
-      <c r="B27" s="34"/>
-      <c r="C27" s="34"/>
-      <c r="D27" s="34"/>
-      <c r="E27" s="34"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="34"/>
-      <c r="H27" s="34"/>
-      <c r="I27" s="34"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A28" s="30">
+      <c r="A28" s="36">
         <v>5</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="35" t="s">
         <v>233</v>
       </c>
       <c r="D28" s="19" t="s">
@@ -8769,9 +8775,9 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="30"/>
-      <c r="B29" s="30"/>
-      <c r="C29" s="32"/>
+      <c r="A29" s="36"/>
+      <c r="B29" s="36"/>
+      <c r="C29" s="35"/>
       <c r="D29" s="19" t="s">
         <v>131</v>
       </c>
@@ -8792,9 +8798,9 @@
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="30"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="32"/>
+      <c r="A30" s="36"/>
+      <c r="B30" s="36"/>
+      <c r="C30" s="35"/>
       <c r="D30" s="19" t="s">
         <v>132</v>
       </c>
@@ -8815,9 +8821,9 @@
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="30"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="32"/>
+      <c r="A31" s="36"/>
+      <c r="B31" s="36"/>
+      <c r="C31" s="35"/>
       <c r="D31" s="19" t="s">
         <v>133</v>
       </c>
@@ -8838,9 +8844,9 @@
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="30"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="32"/>
+      <c r="A32" s="36"/>
+      <c r="B32" s="36"/>
+      <c r="C32" s="35"/>
       <c r="D32" s="19" t="s">
         <v>135</v>
       </c>
@@ -8861,18 +8867,29 @@
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="34"/>
-      <c r="B33" s="34"/>
-      <c r="C33" s="34"/>
-      <c r="D33" s="34"/>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
-      <c r="I33" s="34"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A33:I33"/>
+    <mergeCell ref="B16:B20"/>
+    <mergeCell ref="A16:A20"/>
+    <mergeCell ref="C16:C20"/>
+    <mergeCell ref="C22:C26"/>
+    <mergeCell ref="A21:I21"/>
+    <mergeCell ref="C28:C32"/>
+    <mergeCell ref="B28:B32"/>
+    <mergeCell ref="A28:A32"/>
+    <mergeCell ref="A22:A26"/>
+    <mergeCell ref="B22:B26"/>
     <mergeCell ref="A27:I27"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A2:I2"/>
@@ -8880,21 +8897,10 @@
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="A4:A8"/>
     <mergeCell ref="A9:I9"/>
-    <mergeCell ref="A33:I33"/>
-    <mergeCell ref="B16:B20"/>
-    <mergeCell ref="A16:A20"/>
-    <mergeCell ref="C16:C20"/>
-    <mergeCell ref="C22:C26"/>
     <mergeCell ref="C10:C14"/>
     <mergeCell ref="B10:B14"/>
     <mergeCell ref="A10:A14"/>
-    <mergeCell ref="A21:I21"/>
     <mergeCell ref="A15:I15"/>
-    <mergeCell ref="C28:C32"/>
-    <mergeCell ref="B28:B32"/>
-    <mergeCell ref="A28:A32"/>
-    <mergeCell ref="A22:A26"/>
-    <mergeCell ref="B22:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>